<commit_message>
S4Loader - adding speadsheet of enum translations and associated reader module.
</commit_message>
<xml_diff>
--- a/data/S4Loader_configs/pdt_field_eval_specifications.xlsx
+++ b/data/S4Loader_configs/pdt_field_eval_specifications.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\coding\work\work-flix\data\S4Loader_configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD6E39FF-E7ED-4FA6-B9D1-D09C8D789D21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95CCC91C-E866-4E81-8A6C-80416CC0E33D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" tabRatio="500" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" tabRatio="500" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PDT_Damper" sheetId="1" r:id="rId1"/>
@@ -26,12 +26,24 @@
   <definedNames>
     <definedName name="Characteristics">[1]Characteristics!$A$3:$N$43</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="247">
   <si>
     <t>s4_type</t>
   </si>
@@ -769,6 +781,9 @@
   </si>
   <si>
     <t>80mm</t>
+  </si>
+  <si>
+    <t>asset-status</t>
   </si>
 </sst>
 </file>
@@ -4848,8 +4863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFAEB776-845F-402D-949C-37AF9B4CC451}">
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4919,9 +4934,11 @@
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>246</v>
+      </c>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -5415,7 +5432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA1863E4-1492-41A1-8AD9-960660102BB8}">
   <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="H69" sqref="H69"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
S4Loader fixed a primary key error on meta_pdt_field_value_enums table.
</commit_message>
<xml_diff>
--- a/data/S4Loader_configs/pdt_field_eval_specifications.xlsx
+++ b/data/S4Loader_configs/pdt_field_eval_specifications.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\coding\work\work-flix\data\S4Loader_configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95CCC91C-E866-4E81-8A6C-80416CC0E33D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C691647-7E9F-4D6A-B314-D9F07FF16E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" tabRatio="500" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="673" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PDT_Damper" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,11 @@
     <sheet name="PDT_MotorControlCentre" sheetId="3" r:id="rId3"/>
     <sheet name="PDT_Valves" sheetId="2" r:id="rId4"/>
     <sheet name="PDT_Pressure Transmitter" sheetId="4" r:id="rId5"/>
-    <sheet name="PDT_Flow Transmitter Data" sheetId="6" r:id="rId6"/>
+    <sheet name="PDT_Tank Data" sheetId="7" r:id="rId6"/>
+    <sheet name="PDT_Flow Transmitter Data" sheetId="6" r:id="rId7"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <definedNames>
     <definedName name="Characteristics">[1]Characteristics!$A$3:$N$43</definedName>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="276">
   <si>
     <t>s4_type</t>
   </si>
@@ -784,6 +785,93 @@
   </si>
   <si>
     <t>asset-status</t>
+  </si>
+  <si>
+    <t>Column Material</t>
+  </si>
+  <si>
+    <t>Floor Material</t>
+  </si>
+  <si>
+    <t>Reservoir Covering</t>
+  </si>
+  <si>
+    <t>Roof Material</t>
+  </si>
+  <si>
+    <t>Tank Construction</t>
+  </si>
+  <si>
+    <t>Tank Covering</t>
+  </si>
+  <si>
+    <t>Tank Level</t>
+  </si>
+  <si>
+    <t>Wall Material</t>
+  </si>
+  <si>
+    <t>Dimensions &amp; Weight Data</t>
+  </si>
+  <si>
+    <t>Bottom Water Level (mAOD)</t>
+  </si>
+  <si>
+    <t>Top Water Level (mAOD)</t>
+  </si>
+  <si>
+    <t>Tank Shape</t>
+  </si>
+  <si>
+    <t>Capacity (m3)</t>
+  </si>
+  <si>
+    <t>Diameter (mm)</t>
+  </si>
+  <si>
+    <t>Side Depth (mm)</t>
+  </si>
+  <si>
+    <t>Side Depth Max (mm)</t>
+  </si>
+  <si>
+    <t>Side Depth Min (mm)</t>
+  </si>
+  <si>
+    <t>Top Surface Area (m2)</t>
+  </si>
+  <si>
+    <t>Centre Depth (mm)</t>
+  </si>
+  <si>
+    <t>Length (mm)</t>
+  </si>
+  <si>
+    <t>Major Axis (mm)</t>
+  </si>
+  <si>
+    <t>Minor Axis (mm)</t>
+  </si>
+  <si>
+    <t>Content Type</t>
+  </si>
+  <si>
+    <t>m3</t>
+  </si>
+  <si>
+    <t>m2</t>
+  </si>
+  <si>
+    <t>50.4 m3</t>
+  </si>
+  <si>
+    <t>800 mm</t>
+  </si>
+  <si>
+    <t>35.4 m2</t>
+  </si>
+  <si>
+    <t>4000 mm</t>
   </si>
 </sst>
 </file>
@@ -4863,8 +4951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFAEB776-845F-402D-949C-37AF9B4CC451}">
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5429,11 +5517,754 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECDA521A-C6B9-4F79-9680-60EC00494069}">
+  <dimension ref="A1:F77"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="42.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="6" width="26.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>247</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>248</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>249</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>250</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>251</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>252</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>253</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>254</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>258</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>259</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>260</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>261</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>262</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>263</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>264</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>265</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>266</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>68</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>70</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>72</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>73</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>74</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>77</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>78</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>80</v>
+      </c>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>79</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>269</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA1863E4-1492-41A1-8AD9-960660102BB8}">
   <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="H69" sqref="H69"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61:F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>